<commit_message>
added mutlitple overlaps per condition
</commit_message>
<xml_diff>
--- a/Experimental_Samples.xlsx
+++ b/Experimental_Samples.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="8060" yWindow="920" windowWidth="22540" windowHeight="17440"/>
+    <workbookView xWindow="45440" yWindow="5560" windowWidth="22540" windowHeight="17440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="38">
   <si>
     <t>File1</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Final Stage</t>
   </si>
   <si>
-    <t>Spike Comparison</t>
-  </si>
-  <si>
     <t>Condition</t>
   </si>
   <si>
@@ -90,12 +87,6 @@
     <t>fastq_folder/H3K27ac_inh_Rep1_R2.fastq.gz</t>
   </si>
   <si>
-    <t>H3K27ac</t>
-  </si>
-  <si>
-    <t>Comparison Name</t>
-  </si>
-  <si>
     <t>Sample Number</t>
   </si>
   <si>
@@ -145,6 +136,15 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>Comparisons</t>
+  </si>
+  <si>
+    <t>Spike-in Comparisons</t>
+  </si>
+  <si>
+    <t>H3K27ac_inh, H3_inh</t>
   </si>
 </sst>
 </file>
@@ -507,7 +507,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -518,7 +518,8 @@
     <col min="4" max="4" width="39.1640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="37.6640625" style="2" customWidth="1"/>
     <col min="6" max="6" width="13.1640625" style="2" customWidth="1"/>
-    <col min="7" max="8" width="17.5" style="2" customWidth="1"/>
+    <col min="7" max="7" width="19.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="19.1640625" style="2" customWidth="1"/>
     <col min="9" max="9" width="10.83203125" style="2"/>
     <col min="10" max="10" width="15.6640625" style="2" customWidth="1"/>
     <col min="11" max="16384" width="10.83203125" style="2"/>
@@ -526,13 +527,13 @@
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -544,25 +545,25 @@
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -570,37 +571,37 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="J2" s="2">
         <v>4</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -608,37 +609,37 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="J3" s="2">
         <v>5</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -646,37 +647,34 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="H4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="J4" s="2">
         <v>6</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -684,22 +682,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -707,22 +705,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="K6" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -730,22 +728,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M7" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -753,40 +751,40 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="F8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="J8" s="2">
         <v>8</v>
       </c>
       <c r="K8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="L8" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="M8" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -794,29 +792,29 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="K9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="L9" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="M9" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
updated to bowtie2 option
</commit_message>
<xml_diff>
--- a/Experimental_Samples.xlsx
+++ b/Experimental_Samples.xlsx
@@ -1,37 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28502"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dlk41/Library/Mobile Documents/com~apple~CloudDocs/python_modules/alpha_chrom/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9374468C-3FC1-564E-9875-822FAB211E37}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="45440" yWindow="5560" windowWidth="22540" windowHeight="17440"/>
+    <workbookView xWindow="1380" yWindow="4920" windowWidth="30560" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="48">
   <si>
     <t>File1</t>
   </si>
@@ -39,15 +40,9 @@
     <t>File2</t>
   </si>
   <si>
-    <t>Final Stage</t>
-  </si>
-  <si>
     <t>Condition</t>
   </si>
   <si>
-    <t>H3K27ac_DMSO</t>
-  </si>
-  <si>
     <t>Replicate</t>
   </si>
   <si>
@@ -60,97 +55,133 @@
     <t>Rep3</t>
   </si>
   <si>
-    <t>fastq_folder/H3K27ac_DMSO_Rep1.fastq.gz</t>
-  </si>
-  <si>
-    <t>fastq_folder/H3K27ac_DMSO_Rep2.fastq.gz</t>
-  </si>
-  <si>
-    <t>fastq_folder/H3K27ac_DMSO_Rep3.fastq.gz</t>
-  </si>
-  <si>
-    <t>all</t>
+    <t>Sample Number</t>
+  </si>
+  <si>
+    <t>Genome</t>
+  </si>
+  <si>
+    <t>hg38</t>
+  </si>
+  <si>
+    <t>Sequencer</t>
+  </si>
+  <si>
+    <t>Nextseq</t>
+  </si>
+  <si>
+    <t>HiSeq</t>
+  </si>
+  <si>
+    <t>Input_DMSO</t>
+  </si>
+  <si>
+    <t>H3_inh</t>
+  </si>
+  <si>
+    <t>fastq_folder/Input_DMSO_Rep1.fastq.gz</t>
+  </si>
+  <si>
+    <t>fastq_folder/Input_DMSO_Rep2.fastq.gz</t>
+  </si>
+  <si>
+    <t>fastq_folder/Input_DMSO_Rep3.fastq.gz</t>
+  </si>
+  <si>
+    <t>Background Sample</t>
+  </si>
+  <si>
+    <t>UMI</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Comparisons</t>
+  </si>
+  <si>
+    <t>Spike-in Comparisons</t>
+  </si>
+  <si>
+    <t>macs2</t>
+  </si>
+  <si>
+    <t>Aligner</t>
+  </si>
+  <si>
+    <t>Peak Caller</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>bowtie2</t>
+  </si>
+  <si>
+    <t>bwa</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>TF1</t>
+  </si>
+  <si>
+    <t>bam_folder/TF1.bam</t>
+  </si>
+  <si>
+    <t>fastq_folder/Histone1_DMSO_Rep1.fastq.gz</t>
+  </si>
+  <si>
+    <t>fastq_folder/Histone1_DMSO_Rep2.fastq.gz</t>
+  </si>
+  <si>
+    <t>fastq_folder/Histone1_DMSO_Rep3.fastq.gz</t>
+  </si>
+  <si>
+    <t>fastq_folder/Histone1_inh_Rep1_R1.fastq.gz</t>
+  </si>
+  <si>
+    <t>fastq_folder/Histone1_inh_H3_R1.fastq.gz</t>
+  </si>
+  <si>
+    <t>Histone1_DMSO</t>
+  </si>
+  <si>
+    <t>Histone1_inh</t>
+  </si>
+  <si>
+    <t>TF1_Input</t>
+  </si>
+  <si>
+    <t>bam_folder/TF1_Input.bam</t>
+  </si>
+  <si>
+    <t>fastq_folder/Histone1_inh_Rep1_R2.fastq.gz</t>
+  </si>
+  <si>
+    <t>fastq_folder/Histone1_inh_H3_R2.fastq.gz</t>
+  </si>
+  <si>
+    <t>Histone1_inh, H3_inh</t>
+  </si>
+  <si>
+    <t>ChIP Type</t>
+  </si>
+  <si>
+    <t>histone</t>
   </si>
   <si>
     <t>TF</t>
-  </si>
-  <si>
-    <t>ChIP Type</t>
-  </si>
-  <si>
-    <t>H3K27ac_inh</t>
-  </si>
-  <si>
-    <t>fastq_folder/H3K27ac_inh_Rep1_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>fastq_folder/H3K27ac_inh_Rep1_R2.fastq.gz</t>
-  </si>
-  <si>
-    <t>Sample Number</t>
-  </si>
-  <si>
-    <t>Genome</t>
-  </si>
-  <si>
-    <t>hg38</t>
-  </si>
-  <si>
-    <t>Sequencer</t>
-  </si>
-  <si>
-    <t>Nextseq</t>
-  </si>
-  <si>
-    <t>HiSeq</t>
-  </si>
-  <si>
-    <t>fastq_folder/H3K27ac_inh_H3_R2.fastq.gz</t>
-  </si>
-  <si>
-    <t>fastq_folder/H3K27ac_inh_H3_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>Input_DMSO</t>
-  </si>
-  <si>
-    <t>H3_inh</t>
-  </si>
-  <si>
-    <t>fastq_folder/Input_DMSO_Rep1.fastq.gz</t>
-  </si>
-  <si>
-    <t>fastq_folder/Input_DMSO_Rep2.fastq.gz</t>
-  </si>
-  <si>
-    <t>fastq_folder/Input_DMSO_Rep3.fastq.gz</t>
-  </si>
-  <si>
-    <t>Background Sample</t>
-  </si>
-  <si>
-    <t>UMI</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Comparisons</t>
-  </si>
-  <si>
-    <t>Spike-in Comparisons</t>
-  </si>
-  <si>
-    <t>H3K27ac_inh, H3_inh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -502,12 +533,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -517,23 +548,23 @@
     <col min="3" max="3" width="11.33203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="39.1640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="37.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="13.1640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="19.6640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="19.1640625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="2"/>
-    <col min="10" max="10" width="15.6640625" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="2"/>
+    <col min="6" max="7" width="13.1640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="19.1640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="14.5" style="2" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -542,279 +573,358 @@
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="K1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="D2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" s="2">
+        <v>4</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="2">
-        <v>4</v>
-      </c>
-      <c r="K2" s="2" t="s">
+      <c r="M2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" s="2">
+        <v>39</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K3" s="2">
         <v>5</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K4" s="2">
+        <v>6</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4" s="2">
-        <v>6</v>
-      </c>
-      <c r="K4" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="L5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="L5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="L6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="L7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="F8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K8" s="2">
+        <v>8</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J8" s="2">
-        <v>8</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N8" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="J10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K10" s="2">
+        <v>10</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="L9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>34</v>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>